<commit_message>
* Se suben Métricas
</commit_message>
<xml_diff>
--- a/Cursada/TP3/Planilla de Métricas.xlsx
+++ b/Cursada/TP3/Planilla de Métricas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcabral.DGUIAF\workspace\ProgramacionAvanzada\Clase\TP2\Programa\src\TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alphastrike\Documents\SourceTree\Eclipse\ProgramacionAvanzada\Cursada\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Métricas" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -123,34 +123,37 @@
     <t>TOTALES Desarrollo</t>
   </si>
   <si>
-    <t>metodos clase vector</t>
-  </si>
-  <si>
-    <t>atributos ,metodos equals y get() y set() clase matriz</t>
-  </si>
-  <si>
-    <t>constructores clase matriz</t>
-  </si>
-  <si>
-    <t>metodos clase matriz</t>
-  </si>
-  <si>
-    <t>constructores y atributos clase sel</t>
-  </si>
-  <si>
-    <t>metodos clase sel</t>
-  </si>
-  <si>
-    <t>atributos ,metodos equals,clone y get() y set() clase vector</t>
-  </si>
-  <si>
-    <t>constructores clase vector, toString()</t>
+    <t>Implementación evaluarMSucesivas</t>
+  </si>
+  <si>
+    <t>Lectura de Archivo</t>
+  </si>
+  <si>
+    <t>Implementación toString()</t>
+  </si>
+  <si>
+    <t>Implementación evaluarRecursiva</t>
+  </si>
+  <si>
+    <t>Implementación evaluarRecursivaPar</t>
+  </si>
+  <si>
+    <t>Implementación evaluarProgDinamica</t>
+  </si>
+  <si>
+    <t>Implementación evaluarMejorada</t>
+  </si>
+  <si>
+    <t>Implementación evaluarPow</t>
+  </si>
+  <si>
+    <t>Implementación evaluarHorner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="[h]:mm"/>
@@ -261,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -645,25 +648,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -855,12 +845,26 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -871,44 +875,23 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -918,40 +901,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -962,15 +919,203 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1015,7 +1160,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1054,6 +1199,11 @@
                 <a:srgbClr val="FFC000"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-79F1-40E7-8B25-B4B7B8AF57A3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1063,6 +1213,11 @@
                 <a:srgbClr val="00B0F0"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-79F1-40E7-8B25-B4B7B8AF57A3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1072,6 +1227,11 @@
                 <a:srgbClr val="0066FF"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-79F1-40E7-8B25-B4B7B8AF57A3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1081,6 +1241,11 @@
                 <a:srgbClr val="009900"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-79F1-40E7-8B25-B4B7B8AF57A3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1090,6 +1255,11 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-79F1-40E7-8B25-B4B7B8AF57A3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1099,10 +1269,15 @@
                 <a:srgbClr val="002060"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-79F1-40E7-8B25-B4B7B8AF57A3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$37:$D$42</c:f>
+              <c:f>Métricas!$B$38:$D$43</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1128,31 +1303,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$E$37:$E$42</c:f>
+              <c:f>Métricas!$E$38:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.9444444444444198E-3</c:v>
+                  <c:v>1.2500000000000067E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7361111111111105E-2</c:v>
+                  <c:v>2.430555555555558E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2916666666666641E-2</c:v>
+                  <c:v>2.430555555555558E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1111111111111072E-2</c:v>
+                  <c:v>2.777777777777779E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3194444444444444E-2</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12638888888888902</c:v>
+                  <c:v>0.12569444444444436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-79F1-40E7-8B25-B4B7B8AF57A3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1186,7 +1366,7 @@
           <a:pPr>
             <a:defRPr lang="es-ES"/>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1214,13 +1394,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>9527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1530,17 +1710,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="28" customWidth="1"/>
-    <col min="3" max="11" width="11.42578125" style="28" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="28" customWidth="1"/>
+    <col min="6" max="11" width="11.42578125" style="28" customWidth="1"/>
     <col min="12" max="12" width="13" style="28" customWidth="1"/>
     <col min="13" max="14" width="11.42578125" style="28" customWidth="1"/>
     <col min="15" max="15" width="1.140625" style="21" customWidth="1"/>
@@ -1548,21 +1730,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
     </row>
     <row r="2" spans="1:16" s="10" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="60"/>
@@ -1581,12 +1763,12 @@
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="70"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1627,17 +1809,17 @@
     <row r="5" spans="1:16" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="1">
-        <v>6.9444444444444441E-3</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="C5" s="2">
-        <v>0.4513888888888889</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D5" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="E5" s="52">
         <f>IFERROR(IF(OR(ISBLANK(C5),ISBLANK(D5)),"Completar",IF(D5&gt;=C5,D5-C5,"Error")),"Error")</f>
-        <v>6.9444444444444198E-3</v>
+        <v>1.2500000000000067E-2</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
@@ -1671,12 +1853,12 @@
     </row>
     <row r="7" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="65"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="70"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1717,17 +1899,17 @@
     <row r="9" spans="1:16" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="1">
-        <v>2.7777777777777776E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C9" s="2">
-        <v>0.46180555555555558</v>
+        <v>0.62152777777777779</v>
       </c>
       <c r="D9" s="2">
-        <v>0.47916666666666669</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="E9" s="52">
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
-        <v>1.7361111111111105E-2</v>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="F9" s="67"/>
       <c r="G9" s="67"/>
@@ -1761,12 +1943,12 @@
     </row>
     <row r="11" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -1810,14 +1992,14 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="C13" s="2">
-        <v>0.48541666666666666</v>
+        <v>0.64930555555555558</v>
       </c>
       <c r="D13" s="2">
-        <v>0.5083333333333333</v>
+        <v>0.67361111111111116</v>
       </c>
       <c r="E13" s="52">
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
-        <v>2.2916666666666641E-2</v>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="F13" s="67"/>
       <c r="G13" s="67"/>
@@ -1851,50 +2033,50 @@
     </row>
     <row r="15" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="65"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="70"/>
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:16" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="88"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="90" t="s">
+      <c r="D16" s="75"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="91"/>
-      <c r="H16" s="87" t="s">
+      <c r="G16" s="63"/>
+      <c r="H16" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="88"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="90" t="s">
+      <c r="I16" s="75"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="91"/>
-      <c r="M16" s="87" t="s">
+      <c r="L16" s="63"/>
+      <c r="M16" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="95" t="s">
+      <c r="N16" s="65" t="s">
         <v>2</v>
       </c>
       <c r="O16" s="14"/>
@@ -1902,10 +2084,10 @@
     </row>
     <row r="17" spans="1:16" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="89"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="76"/>
       <c r="F17" s="39" t="s">
         <v>12</v>
       </c>
@@ -1927,37 +2109,36 @@
       <c r="L17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="87"/>
-      <c r="N17" s="95"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="65"/>
       <c r="O17" s="14"/>
       <c r="P17" s="18"/>
     </row>
     <row r="18" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="44">
-        <f>ROW($B18)-16</f>
-        <v>2</v>
-      </c>
-      <c r="C18" s="79" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
+        <v>1</v>
+      </c>
+      <c r="C18" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="77"/>
+      <c r="E18" s="78"/>
       <c r="F18" s="3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G18" s="4">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="H18" s="5">
-        <v>0.50902777777777775</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="I18" s="6">
-        <v>0.51388888888888895</v>
+        <v>0.60138888888888886</v>
       </c>
       <c r="J18" s="53">
-        <f>IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
-        <v>4.8611111111112049E-3</v>
+        <f t="shared" ref="J18:J23" si="0">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
+        <v>4.1666666666666519E-3</v>
       </c>
       <c r="K18" s="7">
         <v>0</v>
@@ -1966,11 +2147,11 @@
         <v>0</v>
       </c>
       <c r="M18" s="9">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="N18" s="54">
         <f>IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
-        <v>4.8611111111112049E-3</v>
+        <v>4.1666666666666519E-3</v>
       </c>
       <c r="O18" s="19"/>
       <c r="P18" s="22"/>
@@ -1978,29 +2159,28 @@
     <row r="19" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="44">
-        <f t="shared" ref="B19:B25" si="0">ROW($B19)-16</f>
-        <v>3</v>
-      </c>
-      <c r="C19" s="79" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="80"/>
+        <v>2</v>
+      </c>
+      <c r="C19" s="77" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="77"/>
+      <c r="E19" s="78"/>
       <c r="F19" s="3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G19" s="4">
-        <v>1.0416666666666666E-2</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="H19" s="5">
-        <v>0.51527777777777783</v>
+        <v>0.60763888888888895</v>
       </c>
       <c r="I19" s="6">
-        <v>0.52083333333333337</v>
+        <v>0.61041666666666672</v>
       </c>
       <c r="J19" s="53">
-        <f t="shared" ref="J19:J23" si="1">IFERROR(IF(OR(ISBLANK(H19),ISBLANK(I19)),"",IF(I19&gt;=H19,I19-H19,"Error")),"Error")</f>
-        <v>5.5555555555555358E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.7777777777777679E-3</v>
       </c>
       <c r="K19" s="7">
         <v>0</v>
@@ -2009,54 +2189,53 @@
         <v>0</v>
       </c>
       <c r="M19" s="9">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N19" s="54">
-        <f t="shared" ref="N19:N25" si="2">IFERROR(IF(OR(J19="",ISBLANK(L19)),"",J19+L19),"Error")</f>
-        <v>5.5555555555555358E-3</v>
+        <f t="shared" ref="N19:N26" si="1">IFERROR(IF(OR(J19="",ISBLANK(L19)),"",J19+L19),"Error")</f>
+        <v>2.7777777777777679E-3</v>
       </c>
       <c r="O19" s="19"/>
       <c r="P19" s="22"/>
     </row>
-    <row r="20" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="44">
+        <v>3</v>
+      </c>
+      <c r="C20" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="77"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="3">
+        <v>25</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.72569444444444453</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="J20" s="53">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C20" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="81"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="3">
-        <v>100</v>
-      </c>
-      <c r="G20" s="4">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0.52152777777777781</v>
-      </c>
-      <c r="I20" s="6">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="J20" s="53">
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="8">
+        <v>0</v>
+      </c>
+      <c r="M20" s="9">
+        <v>14</v>
+      </c>
+      <c r="N20" s="54">
         <f t="shared" si="1"/>
-        <v>3.4027777777777768E-2</v>
-      </c>
-      <c r="K20" s="7">
-        <v>5</v>
-      </c>
-      <c r="L20" s="8">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="M20" s="9">
-        <v>86</v>
-      </c>
-      <c r="N20" s="54">
-        <f t="shared" si="2"/>
-        <v>3.7499999999999992E-2</v>
+        <v>1.041666666666663E-2</v>
       </c>
       <c r="O20" s="19"/>
       <c r="P20" s="22"/>
@@ -2064,42 +2243,41 @@
     <row r="21" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="44">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C21" s="79" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="79"/>
-      <c r="E21" s="80"/>
+        <v>4</v>
+      </c>
+      <c r="C21" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="77"/>
+      <c r="E21" s="78"/>
       <c r="F21" s="3">
         <v>30</v>
       </c>
       <c r="G21" s="4">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="J21" s="53">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K21" s="7">
+        <v>2</v>
+      </c>
+      <c r="L21" s="8">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="H21" s="5">
-        <v>0.5625</v>
-      </c>
-      <c r="I21" s="6">
-        <v>0.56805555555555554</v>
-      </c>
-      <c r="J21" s="53">
+      <c r="M21" s="9">
+        <v>8</v>
+      </c>
+      <c r="N21" s="54">
         <f t="shared" si="1"/>
-        <v>5.5555555555555358E-3</v>
-      </c>
-      <c r="K21" s="7">
-        <v>0</v>
-      </c>
-      <c r="L21" s="8">
-        <v>0</v>
-      </c>
-      <c r="M21" s="9">
-        <v>40</v>
-      </c>
-      <c r="N21" s="54">
-        <f t="shared" si="2"/>
-        <v>5.5555555555555358E-3</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="O21" s="19"/>
       <c r="P21" s="22"/>
@@ -2107,42 +2285,41 @@
     <row r="22" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="44">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C22" s="79" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
+        <v>5</v>
+      </c>
+      <c r="C22" s="77" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="77"/>
+      <c r="E22" s="78"/>
       <c r="F22" s="3">
         <v>20</v>
       </c>
       <c r="G22" s="4">
-        <v>6.9444444444444441E-3</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="H22" s="5">
-        <v>0.56944444444444442</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="I22" s="6">
-        <v>0.57708333333333328</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J22" s="53">
+        <f t="shared" si="0"/>
+        <v>2.4305555555555552E-2</v>
+      </c>
+      <c r="K22" s="7">
+        <v>8</v>
+      </c>
+      <c r="L22" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="M22" s="9">
+        <v>18</v>
+      </c>
+      <c r="N22" s="54">
         <f t="shared" si="1"/>
-        <v>7.6388888888888618E-3</v>
-      </c>
-      <c r="K22" s="7">
-        <v>4</v>
-      </c>
-      <c r="L22" s="8">
-        <v>1.3888888888888889E-3</v>
-      </c>
-      <c r="M22" s="9">
-        <v>13</v>
-      </c>
-      <c r="N22" s="54">
-        <f t="shared" si="2"/>
-        <v>9.0277777777777509E-3</v>
+        <v>3.4722222222222217E-2</v>
       </c>
       <c r="O22" s="19"/>
       <c r="P22" s="22"/>
@@ -2150,42 +2327,41 @@
     <row r="23" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="44">
+        <v>6</v>
+      </c>
+      <c r="C23" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="77"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="3">
+        <v>40</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="J23" s="53">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C23" s="79" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="3">
-        <v>200</v>
-      </c>
-      <c r="G23" s="4">
-        <v>3.125E-2</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0.59375</v>
-      </c>
-      <c r="I23" s="6">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="J23" s="53">
-        <f t="shared" si="1"/>
-        <v>4.5138888888888951E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="K23" s="7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L23" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="M23" s="9">
-        <v>210</v>
+        <v>13</v>
       </c>
       <c r="N23" s="54">
-        <f t="shared" si="2"/>
-        <v>5.2083333333333398E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.7777777777777814E-2</v>
       </c>
       <c r="O23" s="19"/>
       <c r="P23" s="22"/>
@@ -2193,29 +2369,28 @@
     <row r="24" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="44">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C24" s="79" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="79"/>
-      <c r="E24" s="80"/>
+        <v>7</v>
+      </c>
+      <c r="C24" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="77"/>
+      <c r="E24" s="78"/>
       <c r="F24" s="3">
         <v>30</v>
       </c>
       <c r="G24" s="4">
-        <v>1.3888888888888888E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="H24" s="5">
-        <v>0.69861111111111107</v>
+        <v>5.9027777777777783E-2</v>
       </c>
       <c r="I24" s="6">
-        <v>0.71527777777777779</v>
+        <v>6.5972222222222224E-2</v>
       </c>
       <c r="J24" s="53">
         <f>IFERROR(IF(OR(ISBLANK(H24),ISBLANK(I24)),"",IF(I24&gt;=H24,I24-H24,"Error")),"Error")</f>
-        <v>1.6666666666666718E-2</v>
+        <v>6.9444444444444406E-3</v>
       </c>
       <c r="K24" s="7">
         <v>0</v>
@@ -2224,276 +2399,293 @@
         <v>0</v>
       </c>
       <c r="M24" s="9">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="N24" s="54">
-        <f t="shared" si="2"/>
-        <v>1.6666666666666718E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.9444444444444406E-3</v>
       </c>
       <c r="O24" s="19"/>
       <c r="P24" s="22"/>
     </row>
     <row r="25" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="44">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C25" s="79" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="79"/>
-      <c r="E25" s="80"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="77"/>
+      <c r="E25" s="78"/>
       <c r="F25" s="3">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G25" s="4">
-        <v>1.0416666666666666E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="H25" s="5">
-        <v>0.72222222222222221</v>
+        <v>0.44930555555555557</v>
       </c>
       <c r="I25" s="6">
-        <v>0.73055555555555562</v>
+        <v>0.46527777777777773</v>
       </c>
       <c r="J25" s="53">
-        <v>6.9444444444444441E-3</v>
+        <f t="shared" ref="J25:J26" si="2">IFERROR(IF(OR(ISBLANK(H25),ISBLANK(I25)),"",IF(I25&gt;=H25,I25-H25,"Error")),"Error")</f>
+        <v>1.5972222222222165E-2</v>
       </c>
       <c r="K25" s="7">
+        <v>1</v>
+      </c>
+      <c r="L25" s="8">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="M25" s="9">
+        <v>8</v>
+      </c>
+      <c r="N25" s="54"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="22"/>
+    </row>
+    <row r="26" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="44">
+        <v>8</v>
+      </c>
+      <c r="C26" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="77"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="3">
+        <v>25</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="H26" s="5">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="I26" s="6">
+        <v>0.12013888888888889</v>
+      </c>
+      <c r="J26" s="53">
+        <f t="shared" si="2"/>
+        <v>2.9861111111111116E-2</v>
+      </c>
+      <c r="K26" s="7">
         <v>3</v>
       </c>
-      <c r="L25" s="8">
-        <v>1.3888888888888889E-3</v>
-      </c>
-      <c r="M25" s="9">
+      <c r="L26" s="8">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="M26" s="9">
+        <v>8</v>
+      </c>
+      <c r="N26" s="54">
+        <f>IFERROR(IF(OR(J26="",ISBLANK(L26)),"",J26+L26),"Error")</f>
+        <v>3.333333333333334E-2</v>
+      </c>
+      <c r="O26" s="19"/>
+      <c r="P26" s="22"/>
+    </row>
+    <row r="27" spans="1:16" s="27" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="45">
+        <f>IF(SUM(F18:F26)=0,"Completar",SUM(F18:F26))</f>
+        <v>240</v>
+      </c>
+      <c r="G27" s="46">
+        <f>IF(SUM(G18:G26)=0,"Completar",SUM(G18:G26))</f>
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="H27" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="49">
+        <f>IF(OR(COUNTIF(J18:J26,"Error")&gt;0,COUNTIF(J18:J26,"Completar")&gt;0),"Error",IF(SUM(J18:J26)=0,"Completar",SUM(J18:J26)))</f>
+        <v>0.12569444444444436</v>
+      </c>
+      <c r="K27" s="50">
+        <f>SUM(K18:K26)</f>
+        <v>16</v>
+      </c>
+      <c r="L27" s="46">
+        <f>SUM(L18:L26)</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="M27" s="51">
+        <f>IF(SUM(M18:M26)=0,"Completar",SUM(M18:M26))</f>
+        <v>109</v>
+      </c>
+      <c r="N27" s="52">
+        <f>IF(OR(COUNTIF(N18:N26,"Error")&gt;0,COUNTIF(N18:N26,"Completar")&gt;0),"Error",IF(SUM(N18:N26)=0,"Completar",SUM(N18:N26)))</f>
+        <v>0.13402777777777775</v>
+      </c>
+      <c r="O27" s="14"/>
+      <c r="P27" s="26"/>
+    </row>
+    <row r="28" spans="1:16" s="24" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+    </row>
+    <row r="29" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="11"/>
+    </row>
+    <row r="30" spans="1:16" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="18"/>
+    </row>
+    <row r="31" spans="1:16" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="E31" s="52">
+        <f>IFERROR(IF(OR(ISBLANK(C31),ISBLANK(D31)),"Completar",IF(D31&gt;=C31,D31-C31,"Error")),"Error")</f>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="22"/>
+    </row>
+    <row r="32" spans="1:16" s="24" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="N25" s="54">
-        <f t="shared" si="2"/>
-        <v>8.3333333333333332E-3</v>
-      </c>
-      <c r="O25" s="19"/>
-      <c r="P25" s="22"/>
-    </row>
-    <row r="26" spans="1:16" s="27" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="92" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="93"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="94"/>
-      <c r="F26" s="45">
-        <f>IF(SUM(F18:F25)=0,"Completar",SUM(F18:F25))</f>
-        <v>444</v>
-      </c>
-      <c r="G26" s="46">
-        <f>IF(SUM(G18:G25)=0,"Completar",SUM(G18:G25))</f>
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="H26" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="J26" s="49">
-        <f>IF(OR(COUNTIF(J18:J25,"Error")&gt;0,COUNTIF(J18:J25,"Completar")&gt;0),"Error",IF(SUM(J18:J25)=0,"Completar",SUM(J18:J25)))</f>
-        <v>0.12638888888888902</v>
-      </c>
-      <c r="K26" s="50">
-        <f>SUM(K18:K25)</f>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="70"/>
+    </row>
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="L26" s="46">
-        <f>SUM(L18:L25)</f>
-        <v>1.3194444444444444E-2</v>
-      </c>
-      <c r="M26" s="51">
-        <f>IF(SUM(M18:M25)=0,"Completar",SUM(M18:M25))</f>
-        <v>435</v>
-      </c>
-      <c r="N26" s="52">
-        <f>IF(OR(COUNTIF(N18:N25,"Error")&gt;0,COUNTIF(N18:N25,"Completar")&gt;0),"Error",IF(SUM(N18:N25)=0,"Completar",SUM(N18:N25)))</f>
-        <v>0.13958333333333348</v>
-      </c>
-      <c r="O26" s="14"/>
-      <c r="P26" s="26"/>
-    </row>
-    <row r="27" spans="1:16" s="24" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-    </row>
-    <row r="28" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="11"/>
-    </row>
-    <row r="29" spans="1:16" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="56" t="s">
-        <v>2</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="18"/>
-    </row>
-    <row r="30" spans="1:16" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
-      <c r="B30" s="1">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0.75694444444444453</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.7680555555555556</v>
-      </c>
-      <c r="E30" s="52">
-        <f>IFERROR(IF(OR(ISBLANK(C30),ISBLANK(D30)),"Completar",IF(D30&gt;=C30,D30-C30,"Error")),"Error")</f>
-        <v>1.1111111111111072E-2</v>
-      </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="22"/>
-    </row>
-    <row r="31" spans="1:16" s="24" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="65"/>
-    </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="83">
-        <f>M26</f>
-        <v>435</v>
-      </c>
-      <c r="F33" s="84"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="31"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="70" t="s">
+      <c r="C34" s="80"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="73">
+        <f>M27</f>
+        <v>109</v>
+      </c>
+      <c r="F34" s="74"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="31"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="71"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="85">
-        <f>IF(M26="Completar","Completar",IFERROR(M26/(N26*24),"Error"))</f>
-        <v>129.85074626865659</v>
-      </c>
-      <c r="F34" s="86"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="34"/>
-    </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="71"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="83">
-        <f>IF(K26=0,0,IFERROR(ROUNDUP(K26/(M26/100),0),"Error"))</f>
-        <v>6</v>
-      </c>
-      <c r="F35" s="84"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="71">
+        <f>IF(M27="Completar","Completar",IFERROR(M27/(N27*24),"Error"))</f>
+        <v>33.886010362694307</v>
+      </c>
+      <c r="F35" s="72"/>
       <c r="G35" s="32"/>
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
@@ -2504,16 +2696,16 @@
       <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="68">
-        <f>IF(K26=0,0,IFERROR(K26/M26,"Error"))</f>
-        <v>5.057471264367816E-2</v>
-      </c>
-      <c r="F36" s="69"/>
+      <c r="B36" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="80"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="73">
+        <f>IF(K27=0,0,IFERROR(ROUNDUP(K27/(M27/100),0),"Error"))</f>
+        <v>15</v>
+      </c>
+      <c r="F36" s="74"/>
       <c r="G36" s="32"/>
       <c r="H36" s="33"/>
       <c r="I36" s="33"/>
@@ -2524,19 +2716,16 @@
       <c r="N36" s="34"/>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="57">
-        <f>E5</f>
-        <v>6.9444444444444198E-3</v>
-      </c>
-      <c r="F37" s="58">
-        <f>IF(E37="Completar",E37,IFERROR(E37/$E$43,"Error"))</f>
-        <v>3.5087719298245487E-2</v>
-      </c>
+      <c r="B37" s="79" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="80"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="85">
+        <f>IF(K27=0,0,IFERROR(K27/M27,"Error"))</f>
+        <v>0.14678899082568808</v>
+      </c>
+      <c r="F37" s="86"/>
       <c r="G37" s="32"/>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -2547,18 +2736,18 @@
       <c r="N37" s="34"/>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="72"/>
+      <c r="B38" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="80"/>
+      <c r="D38" s="81"/>
       <c r="E38" s="57">
-        <f>E9</f>
-        <v>1.7361111111111105E-2</v>
+        <f>E5</f>
+        <v>1.2500000000000067E-2</v>
       </c>
       <c r="F38" s="58">
-        <f>IF(E38="Completar",E38,IFERROR(E38/$E$43,"Error"))</f>
-        <v>8.7719298245614002E-2</v>
+        <f>IF(E38="Completar",E38,IFERROR(E38/$E$44,"Error"))</f>
+        <v>5.1575931232091962E-2</v>
       </c>
       <c r="G38" s="32"/>
       <c r="H38" s="33"/>
@@ -2570,18 +2759,18 @@
       <c r="N38" s="34"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="72"/>
+      <c r="B39" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="80"/>
+      <c r="D39" s="81"/>
       <c r="E39" s="57">
-        <f>E13</f>
-        <v>2.2916666666666641E-2</v>
+        <f>E9</f>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="F39" s="58">
-        <f t="shared" ref="F39" si="3">IF(E39="Completar",E39,IFERROR(E39/$E$43,"Error"))</f>
-        <v>0.11578947368421039</v>
+        <f>IF(E39="Completar",E39,IFERROR(E39/$E$44,"Error"))</f>
+        <v>0.10028653295128949</v>
       </c>
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
@@ -2593,18 +2782,18 @@
       <c r="N39" s="34"/>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="71"/>
-      <c r="D40" s="72"/>
+      <c r="B40" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="80"/>
+      <c r="D40" s="81"/>
       <c r="E40" s="57">
-        <f>E30</f>
-        <v>1.1111111111111072E-2</v>
+        <f>E13</f>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="F40" s="58">
-        <f>IF(E40="Completar",E40,IFERROR(E40/$E$43,"Error"))</f>
-        <v>5.6140350877192775E-2</v>
+        <f t="shared" ref="F40" si="3">IF(E40="Completar",E40,IFERROR(E40/$E$44,"Error"))</f>
+        <v>0.10028653295128949</v>
       </c>
       <c r="G40" s="32"/>
       <c r="H40" s="33"/>
@@ -2616,18 +2805,18 @@
       <c r="N40" s="34"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="72"/>
+      <c r="B41" s="79" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="80"/>
+      <c r="D41" s="81"/>
       <c r="E41" s="57">
-        <f>L26</f>
-        <v>1.3194444444444444E-2</v>
+        <f>E31</f>
+        <v>2.777777777777779E-2</v>
       </c>
       <c r="F41" s="58">
-        <f>IF(E41="Completar",E41,IFERROR(E41/$E$43,"Completar"))</f>
-        <v>6.6666666666666666E-2</v>
+        <f>IF(E41="Completar",E41,IFERROR(E41/$E$44,"Error"))</f>
+        <v>0.11461318051575935</v>
       </c>
       <c r="G41" s="32"/>
       <c r="H41" s="33"/>
@@ -2639,18 +2828,18 @@
       <c r="N41" s="34"/>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="71"/>
-      <c r="D42" s="72"/>
+      <c r="B42" s="79" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="80"/>
+      <c r="D42" s="81"/>
       <c r="E42" s="57">
-        <f>J26</f>
-        <v>0.12638888888888902</v>
+        <f>L27</f>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="F42" s="58">
-        <f>IF(E42="Completar",E42,IFERROR(E42/$E$43,"Completar"))</f>
-        <v>0.63859649122807083</v>
+        <f>IF(E42="Completar",E42,IFERROR(E42/$E$44,"Completar"))</f>
+        <v>0.11461318051575929</v>
       </c>
       <c r="G42" s="32"/>
       <c r="H42" s="33"/>
@@ -2661,31 +2850,53 @@
       <c r="M42" s="33"/>
       <c r="N42" s="34"/>
     </row>
-    <row r="43" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="76" t="s">
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="80"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="57">
+        <f>J27</f>
+        <v>0.12569444444444436</v>
+      </c>
+      <c r="F43" s="58">
+        <f>IF(E43="Completar",E43,IFERROR(E43/$E$44,"Completar"))</f>
+        <v>0.51862464183381052</v>
+      </c>
+      <c r="G43" s="32"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="34"/>
+    </row>
+    <row r="44" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="77"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="73">
-        <f>IF(COUNTIF(E37:E42,"Error")&gt;0,"Error",IF(SUM(E37:E42)=0,"Completar",SUM(E37:E42)))</f>
-        <v>0.19791666666666669</v>
-      </c>
-      <c r="F43" s="74"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="37"/>
-    </row>
-    <row r="44" spans="1:15" s="38" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="O44" s="21"/>
-    </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="87">
+        <f>IF(COUNTIF(E38:E43,"Error")&gt;0,"Error",IF(SUM(E38:E43)=0,"Completar",SUM(E38:E43)))</f>
+        <v>0.24236111111111114</v>
+      </c>
+      <c r="F44" s="88"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="37"/>
+    </row>
+    <row r="45" spans="1:15" s="38" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="O45" s="21"/>
+    </row>
     <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
@@ -2709,46 +2920,11 @@
     <row r="66" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="67" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="68" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="69" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <mergeCells count="44">
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
+  <mergeCells count="45">
     <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="B32:N32"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E33:F33"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:N1"/>
     <mergeCell ref="B11:E11"/>
@@ -2756,12 +2932,105 @@
     <mergeCell ref="F13:N13"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B33:N33"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B15:N15"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:B1048576 D1:XFD1048576 C3:C1048576">
+  <conditionalFormatting sqref="A1:B1048576 D1:XFD17 C3:C18 C27:XFD1048576 F24:XFD26 D18:I18 J18:XFD23 F19:I23">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="25" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:E19">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:E25">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:E20">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:E21">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:E22">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:E23">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:E26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>